<commit_message>
Reusable in Working condition
</commit_message>
<xml_diff>
--- a/KeywordDriven_Framework/ExcelTestFiles/Object Repository.xlsx
+++ b/KeywordDriven_Framework/ExcelTestFiles/Object Repository.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Reservation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Locator Value</t>
   </si>
@@ -87,7 +87,31 @@
     <t>fromMonth</t>
   </si>
   <si>
-    <t>Departing On</t>
+    <t>Departing On Month</t>
+  </si>
+  <si>
+    <t>fromDay</t>
+  </si>
+  <si>
+    <t>Departing On Date</t>
+  </si>
+  <si>
+    <t>Arriving In</t>
+  </si>
+  <si>
+    <t>toPort</t>
+  </si>
+  <si>
+    <t>Returning Month</t>
+  </si>
+  <si>
+    <t>toMonth</t>
+  </si>
+  <si>
+    <t>toDay</t>
+  </si>
+  <si>
+    <t>Returning Date</t>
   </si>
 </sst>
 </file>
@@ -153,11 +177,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -442,7 +467,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,10 +548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +560,7 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -615,6 +640,66 @@
       </c>
       <c r="E5" s="1"/>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>